<commit_message>
v0.2 BackTester and v2.0 DataDownloader.
</commit_message>
<xml_diff>
--- a/ScoringConfig.xlsx
+++ b/ScoringConfig.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholastorres/Coding/HAVEN-MK-3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholastorres/Coding/Haven-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF281A0-E945-5A43-93C2-696B5B525691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF2A163-797B-5A43-8F31-1FC9DD74F502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="14700" windowHeight="18360" xr2:uid="{4C302A0A-2DAA-6D4A-B671-BE37219EA0D1}"/>
   </bookViews>
@@ -576,7 +576,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="1">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>